<commit_message>
runtime and sensor correction etc.
</commit_message>
<xml_diff>
--- a/AddrTag-4X.B.xlsx
+++ b/AddrTag-4X.B.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyCloud\TQWorking\Cheetah600\Cheetah600_LCD\Cheetah600\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F39FF5-FAFE-4D9B-B9E0-50C6FDAC707F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865F22E6-FEC9-444D-9D9E-A60855A4F937}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="127">
   <si>
     <t>AddrTag Lib</t>
   </si>
@@ -58,15 +58,6 @@
     <t>备注</t>
   </si>
   <si>
-    <t>循环泵</t>
-  </si>
-  <si>
-    <t>气泵</t>
-  </si>
-  <si>
-    <t>UV</t>
-  </si>
-  <si>
     <t>state_DO_SF_EV_BPOS</t>
   </si>
   <si>
@@ -103,9 +94,6 @@
     <t>state_DO_COMP2_BPOS</t>
   </si>
   <si>
-    <t>state_DO_HOTBYPASS_BPOS</t>
-  </si>
-  <si>
     <t>state_DO_RELL_BPOS</t>
   </si>
   <si>
@@ -143,9 +131,6 @@
   </si>
   <si>
     <t>state_DO_LED_ORANGE_BPOS</t>
-  </si>
-  <si>
-    <t>state_DO_RSV_BPOS_3</t>
   </si>
   <si>
     <t>state_DO_ALARM_BPOS</t>
@@ -179,60 +164,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>沉淀滤芯电磁阀</t>
-  </si>
-  <si>
-    <t>活性炭滤芯电磁阀</t>
-  </si>
-  <si>
-    <t>饮水箱进水</t>
-  </si>
-  <si>
-    <t>循环支路</t>
-  </si>
-  <si>
-    <t>沉淀杯清洗</t>
-  </si>
-  <si>
-    <t>膨胀水箱</t>
-  </si>
-  <si>
-    <t>冰水阀</t>
-  </si>
-  <si>
-    <t>压机1启动</t>
-  </si>
-  <si>
-    <t>压机2</t>
-  </si>
-  <si>
-    <t>热气旁通</t>
-  </si>
-  <si>
-    <t>转轮</t>
-  </si>
-  <si>
-    <t>转轮电加热</t>
-  </si>
-  <si>
-    <t>常温水</t>
-  </si>
-  <si>
-    <t>冰水</t>
-  </si>
-  <si>
-    <t>预留</t>
-  </si>
-  <si>
-    <t>绿灯</t>
-  </si>
-  <si>
-    <t>红灯</t>
-  </si>
-  <si>
-    <t>橙灯</t>
-  </si>
-  <si>
     <t>DI 源水箱高水位</t>
   </si>
   <si>
@@ -388,6 +319,96 @@
   <si>
     <t>756.00</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>state_DO_HOTBYPASS1_BPOS</t>
+  </si>
+  <si>
+    <t>state_DO_HOTBYPASS2_BPOS</t>
+  </si>
+  <si>
+    <t>DO 沉淀滤芯电磁阀</t>
+  </si>
+  <si>
+    <t>DO 活性炭滤芯电磁阀</t>
+  </si>
+  <si>
+    <t>DO 饮水箱进水</t>
+  </si>
+  <si>
+    <t>DO 循环支路</t>
+  </si>
+  <si>
+    <t>DO 沉淀杯清洗</t>
+  </si>
+  <si>
+    <t>DO 膨胀水箱</t>
+  </si>
+  <si>
+    <t>DO 冰水阀</t>
+  </si>
+  <si>
+    <t>DO 循环泵</t>
+  </si>
+  <si>
+    <t>DO 气泵</t>
+  </si>
+  <si>
+    <t>DO UV</t>
+  </si>
+  <si>
+    <t>DO 压机1启动</t>
+  </si>
+  <si>
+    <t>DO 压机2</t>
+  </si>
+  <si>
+    <t>DO 热气旁通</t>
+  </si>
+  <si>
+    <t>DO 热气旁通2</t>
+  </si>
+  <si>
+    <t>DO 转轮</t>
+  </si>
+  <si>
+    <t>DO 转轮电加热</t>
+  </si>
+  <si>
+    <t>DO 常温水</t>
+  </si>
+  <si>
+    <t>DO 冰水</t>
+  </si>
+  <si>
+    <t>DO 预留1</t>
+  </si>
+  <si>
+    <t>DO 预留</t>
+  </si>
+  <si>
+    <t>DO 绿灯</t>
+  </si>
+  <si>
+    <t>DO 红灯</t>
+  </si>
+  <si>
+    <t>DO 橙灯</t>
+  </si>
+  <si>
+    <t>DO 预留2</t>
+  </si>
+  <si>
+    <t>DO 预留5</t>
+  </si>
+  <si>
+    <t>DO 预留6</t>
+  </si>
+  <si>
+    <t>DO 预留7</t>
+  </si>
+  <si>
+    <t>DO 预留8</t>
   </si>
 </sst>
 </file>
@@ -1345,7 +1366,7 @@
   <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A65"/>
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1395,7 +1416,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1410,7 +1431,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -1422,12 +1443,12 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>51</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1454,12 +1475,12 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>52</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1486,12 +1507,12 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>53</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1518,12 +1539,12 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1550,12 +1571,12 @@
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1582,12 +1603,12 @@
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>56</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1614,12 +1635,12 @@
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1646,12 +1667,12 @@
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>12</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1678,12 +1699,12 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1710,12 +1731,12 @@
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -1730,7 +1751,7 @@
         <v>6</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -1742,12 +1763,12 @@
         <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>58</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -1774,12 +1795,12 @@
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>97</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1806,12 +1827,12 @@
         <v>0</v>
       </c>
       <c r="J15" t="s">
-        <v>60</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>98</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -1838,12 +1859,12 @@
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>61</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -1870,12 +1891,12 @@
         <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>62</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -1902,12 +1923,12 @@
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>63</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -1922,7 +1943,7 @@
         <v>6</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -1934,12 +1955,12 @@
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>64</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -1966,12 +1987,12 @@
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>65</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -1998,12 +2019,12 @@
         <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>65</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -2030,12 +2051,12 @@
         <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>65</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -2062,12 +2083,12 @@
         <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>65</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -2094,12 +2115,12 @@
         <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>65</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -2126,12 +2147,12 @@
         <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>65</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -2158,12 +2179,12 @@
         <v>0</v>
       </c>
       <c r="J26" t="s">
-        <v>66</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -2190,12 +2211,12 @@
         <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>67</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -2222,12 +2243,12 @@
         <v>0</v>
       </c>
       <c r="J28" t="s">
-        <v>68</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -2242,7 +2263,7 @@
         <v>6</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -2254,12 +2275,12 @@
         <v>0</v>
       </c>
       <c r="J29" t="s">
-        <v>65</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -2286,12 +2307,12 @@
         <v>0</v>
       </c>
       <c r="J30" t="s">
-        <v>65</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -2318,12 +2339,12 @@
         <v>0</v>
       </c>
       <c r="J31" t="s">
-        <v>65</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -2350,12 +2371,12 @@
         <v>0</v>
       </c>
       <c r="J32" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -2382,12 +2403,12 @@
         <v>0</v>
       </c>
       <c r="J33" t="s">
-        <v>65</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -2414,12 +2435,12 @@
         <v>0</v>
       </c>
       <c r="J34" t="s">
-        <v>65</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -2434,7 +2455,7 @@
         <v>6</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -2446,12 +2467,12 @@
         <v>0</v>
       </c>
       <c r="J35" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -2478,12 +2499,12 @@
         <v>0</v>
       </c>
       <c r="J36" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -2510,12 +2531,12 @@
         <v>0</v>
       </c>
       <c r="J37" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -2542,12 +2563,12 @@
         <v>0</v>
       </c>
       <c r="J38" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -2574,12 +2595,12 @@
         <v>0</v>
       </c>
       <c r="J39" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -2606,12 +2627,12 @@
         <v>0</v>
       </c>
       <c r="J40" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -2638,12 +2659,12 @@
         <v>0</v>
       </c>
       <c r="J41" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -2670,12 +2691,12 @@
         <v>0</v>
       </c>
       <c r="J42" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -2702,12 +2723,12 @@
         <v>0</v>
       </c>
       <c r="J43" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -2734,12 +2755,12 @@
         <v>0</v>
       </c>
       <c r="J44" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -2754,7 +2775,7 @@
         <v>6</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -2766,12 +2787,12 @@
         <v>0</v>
       </c>
       <c r="J45" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -2798,12 +2819,12 @@
         <v>0</v>
       </c>
       <c r="J46" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -2830,12 +2851,12 @@
         <v>0</v>
       </c>
       <c r="J47" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -2862,12 +2883,12 @@
         <v>0</v>
       </c>
       <c r="J48" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -2894,12 +2915,12 @@
         <v>0</v>
       </c>
       <c r="J49" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -2926,12 +2947,12 @@
         <v>0</v>
       </c>
       <c r="J50" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -2946,7 +2967,7 @@
         <v>6</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="G51">
         <v>0</v>
@@ -2958,12 +2979,12 @@
         <v>0</v>
       </c>
       <c r="J51" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -2990,12 +3011,12 @@
         <v>0</v>
       </c>
       <c r="J52" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -3022,12 +3043,12 @@
         <v>0</v>
       </c>
       <c r="J53" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -3054,12 +3075,12 @@
         <v>0</v>
       </c>
       <c r="J54" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -3086,12 +3107,12 @@
         <v>0</v>
       </c>
       <c r="J55" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -3118,12 +3139,12 @@
         <v>0</v>
       </c>
       <c r="J56" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -3150,12 +3171,12 @@
         <v>0</v>
       </c>
       <c r="J57" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -3182,7 +3203,7 @@
         <v>0</v>
       </c>
       <c r="J58" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>